<commit_message>
Further experiments with params tuning and model redesign
</commit_message>
<xml_diff>
--- a/notebooks/params.xlsx
+++ b/notebooks/params.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filipwojcik/projects/deepautorec_paper/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982BFF34-B48F-3142-93E8-06F606B95E55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCE553B-B301-EA40-9CC9-7E7DD50DFE2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="0" windowWidth="28240" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$S$24</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="70">
   <si>
     <t>inputs dense</t>
   </si>
@@ -212,6 +215,24 @@
   </si>
   <si>
     <t>0.3913579</t>
+  </si>
+  <si>
+    <t>0.3841</t>
+  </si>
+  <si>
+    <t>0.397</t>
+  </si>
+  <si>
+    <t>0.3804</t>
+  </si>
+  <si>
+    <t>0.394</t>
+  </si>
+  <si>
+    <t>0.3781</t>
+  </si>
+  <si>
+    <t>0.386748</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
@@ -1179,12 +1200,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="1">
-        <v>8</v>
+    <row r="2" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4">
+        <v>32</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -1201,11 +1222,11 @@
       <c r="G2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1">
-        <v>8</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4</v>
+      <c r="H2" s="4">
+        <v>16</v>
+      </c>
+      <c r="I2" s="4">
+        <v>8</v>
       </c>
       <c r="J2" s="1">
         <v>0</v>
@@ -1223,13 +1244,13 @@
         <v>52</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1249,7 +1270,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -1276,10 +1297,10 @@
         <v>52</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>21</v>
@@ -1322,11 +1343,8 @@
       <c r="L4" s="1">
         <v>16</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>25</v>
+      <c r="N4" s="1">
+        <v>0</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>52</v>
@@ -1335,7 +1353,7 @@
         <v>22</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>21</v>
@@ -1348,8 +1366,8 @@
       <c r="B5" s="1">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>27</v>
+      <c r="C5" s="1">
+        <v>0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>17</v>
@@ -1358,7 +1376,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="1">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
@@ -1378,20 +1396,23 @@
       <c r="L5" s="1">
         <v>16</v>
       </c>
-      <c r="N5" s="1">
-        <v>0</v>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1411,7 +1432,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>18</v>
@@ -1431,23 +1452,20 @@
       <c r="L6" s="1">
         <v>16</v>
       </c>
-      <c r="M6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>25</v>
+      <c r="N6" s="1">
+        <v>0</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1457,8 +1475,8 @@
       <c r="B7" s="1">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
-        <v>0</v>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>17</v>
@@ -1494,13 +1512,13 @@
         <v>52</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1532,7 +1550,7 @@
         <v>4</v>
       </c>
       <c r="J8" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -1553,10 +1571,10 @@
         <v>22</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1576,7 +1594,7 @@
         <v>17</v>
       </c>
       <c r="F9" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>18</v>
@@ -1585,7 +1603,7 @@
         <v>8</v>
       </c>
       <c r="I9" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J9" s="1">
         <v>0</v>
@@ -1596,11 +1614,8 @@
       <c r="L9" s="1">
         <v>16</v>
       </c>
-      <c r="M9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>25</v>
+      <c r="N9" s="1">
+        <v>0</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>52</v>
@@ -1609,10 +1624,10 @@
         <v>22</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1632,7 +1647,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="1">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>18</v>
@@ -1644,7 +1659,7 @@
         <v>4</v>
       </c>
       <c r="J10" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K10" s="1">
         <v>0</v>
@@ -1665,10 +1680,10 @@
         <v>22</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1688,16 +1703,16 @@
         <v>17</v>
       </c>
       <c r="F11" s="1">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H11" s="1">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="I11" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
@@ -1706,13 +1721,10 @@
         <v>0</v>
       </c>
       <c r="L11" s="1">
-        <v>16</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
+      </c>
+      <c r="N11" s="1">
+        <v>0</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>52</v>
@@ -1721,21 +1733,21 @@
         <v>22</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" s="1">
-        <v>8</v>
-      </c>
-      <c r="C12" s="1">
-        <v>0</v>
+    <row r="12" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="6">
+        <v>32</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>17</v>
@@ -1744,30 +1756,30 @@
         <v>17</v>
       </c>
       <c r="F12" s="1">
-        <v>15</v>
-      </c>
-      <c r="G12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="1">
-        <v>4</v>
-      </c>
-      <c r="I12" s="1">
-        <v>2</v>
+      <c r="H12" s="6">
+        <v>16</v>
+      </c>
+      <c r="I12" s="6">
+        <v>8</v>
       </c>
       <c r="J12" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="1">
-        <v>0</v>
+      <c r="K12" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="L12" s="1">
         <v>16</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O12" s="1" t="s">
@@ -1777,66 +1789,64 @@
         <v>22</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>39</v>
+        <v>68</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="1">
-        <v>8</v>
-      </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1">
-        <v>15</v>
-      </c>
-      <c r="G13" s="1" t="s">
+    <row r="13" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="6">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="6">
+        <v>30</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="1">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1">
-        <v>4</v>
-      </c>
-      <c r="J13" s="1">
-        <v>0</v>
-      </c>
-      <c r="K13" s="1">
-        <v>0</v>
-      </c>
-      <c r="L13" s="1">
-        <v>16</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="O13" s="1" t="s">
+      <c r="H13" s="4">
+        <v>32</v>
+      </c>
+      <c r="I13" s="4">
+        <v>16</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="6">
+        <v>0</v>
+      </c>
+      <c r="L13" s="6">
+        <v>16</v>
+      </c>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6">
+        <v>0</v>
+      </c>
+      <c r="O13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1856,7 +1866,7 @@
         <v>17</v>
       </c>
       <c r="F14" s="1">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>18</v>
@@ -1865,7 +1875,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -1876,20 +1886,23 @@
       <c r="L14" s="1">
         <v>16</v>
       </c>
-      <c r="N14" s="1">
-        <v>0</v>
+      <c r="M14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>52</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -1909,7 +1922,7 @@
         <v>17</v>
       </c>
       <c r="F15" s="1">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>18</v>
@@ -1927,10 +1940,13 @@
         <v>0</v>
       </c>
       <c r="L15" s="1">
-        <v>32</v>
-      </c>
-      <c r="N15" s="1">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>52</v>
@@ -1939,73 +1955,74 @@
         <v>22</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="6">
         <v>32</v>
       </c>
-      <c r="C16" s="1">
-        <v>0</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="1">
+      <c r="C16" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="6">
         <v>30</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="4">
-        <v>16</v>
-      </c>
-      <c r="I16" s="4">
-        <v>8</v>
-      </c>
-      <c r="J16" s="1">
-        <v>0</v>
-      </c>
-      <c r="K16" s="1">
-        <v>0</v>
-      </c>
-      <c r="L16" s="1">
-        <v>16</v>
-      </c>
-      <c r="N16" s="1">
+      <c r="H16" s="6">
+        <v>16</v>
+      </c>
+      <c r="I16" s="6">
+        <v>8</v>
+      </c>
+      <c r="J16" s="6">
+        <v>0</v>
+      </c>
+      <c r="K16" s="6">
+        <v>0</v>
+      </c>
+      <c r="L16" s="6">
+        <v>16</v>
+      </c>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6">
         <v>0</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="6">
-        <v>32</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="B17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="6" t="s">
@@ -2021,10 +2038,10 @@
         <v>18</v>
       </c>
       <c r="H17" s="6">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I17" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J17" s="6">
         <v>0</v>
@@ -2039,25 +2056,25 @@
       <c r="N17" s="6">
         <v>0</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="6" t="s">
         <v>52</v>
       </c>
       <c r="P17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="6">
-        <v>32</v>
+      <c r="B18" s="4">
+        <v>16</v>
       </c>
       <c r="C18" s="7" t="s">
         <v>48</v>
@@ -2075,10 +2092,10 @@
         <v>18</v>
       </c>
       <c r="H18" s="6">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="I18" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J18" s="6">
         <v>0</v>
@@ -2093,17 +2110,17 @@
       <c r="N18" s="6">
         <v>0</v>
       </c>
-      <c r="O18" s="4" t="s">
-        <v>53</v>
+      <c r="O18" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="P18" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:18" ht="34" x14ac:dyDescent="0.2">
@@ -2128,11 +2145,11 @@
       <c r="G19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="4">
-        <v>32</v>
-      </c>
-      <c r="I19" s="4">
-        <v>16</v>
+      <c r="H19" s="6">
+        <v>16</v>
+      </c>
+      <c r="I19" s="6">
+        <v>8</v>
       </c>
       <c r="J19" s="6">
         <v>0</v>
@@ -2148,80 +2165,82 @@
         <v>0</v>
       </c>
       <c r="O19" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P19" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" s="4">
-        <v>16</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="6">
-        <v>30</v>
-      </c>
-      <c r="G20" s="6" t="s">
+    <row r="20" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" s="1">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="6">
-        <v>32</v>
-      </c>
-      <c r="I20" s="6">
-        <v>16</v>
-      </c>
-      <c r="J20" s="6">
-        <v>0</v>
-      </c>
-      <c r="K20" s="6">
-        <v>0</v>
-      </c>
-      <c r="L20" s="6">
-        <v>16</v>
-      </c>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6">
-        <v>0</v>
-      </c>
-      <c r="O20" s="6" t="s">
+      <c r="H20" s="1">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1">
+        <v>8</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0</v>
+      </c>
+      <c r="L20" s="1">
+        <v>16</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="6" t="s">
+      <c r="P20" s="1" t="s">
         <v>22</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="4">
+        <v>16</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2233,13 +2252,13 @@
       <c r="F21" s="6">
         <v>30</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H21" s="6">
+      <c r="G21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="1">
         <v>32</v>
       </c>
-      <c r="I21" s="6">
+      <c r="I21" s="1">
         <v>16</v>
       </c>
       <c r="J21" s="6">
@@ -2262,67 +2281,236 @@
         <v>22</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:18" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="4">
-        <v>16</v>
-      </c>
-      <c r="C22" s="1" t="s">
+      <c r="B22" s="6">
+        <v>32</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="6">
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1">
         <v>30</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="6">
+        <v>16</v>
+      </c>
+      <c r="I22" s="6">
+        <v>8</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L22" s="1">
+        <v>16</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="6">
         <v>32</v>
       </c>
-      <c r="I22" s="1">
-        <v>16</v>
-      </c>
-      <c r="J22" s="6">
-        <v>0</v>
-      </c>
-      <c r="K22" s="6">
-        <v>0</v>
-      </c>
-      <c r="L22" s="6">
-        <v>16</v>
-      </c>
-      <c r="M22" s="6"/>
-      <c r="N22" s="6">
-        <v>0</v>
-      </c>
-      <c r="O22" s="6" t="s">
+      <c r="C23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1">
+        <v>30</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="6">
+        <v>16</v>
+      </c>
+      <c r="I23" s="6">
+        <v>8</v>
+      </c>
+      <c r="J23" s="1">
+        <v>0</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L23" s="1">
+        <v>16</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0</v>
+      </c>
+      <c r="O23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P22" s="6" t="s">
+      <c r="P23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>63</v>
+      <c r="Q23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="1">
+        <v>8</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24" s="1">
+        <v>4</v>
+      </c>
+      <c r="I24" s="1">
+        <v>2</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24" s="1">
+        <v>16</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1">
+        <v>15</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="1">
+        <v>16</v>
+      </c>
+      <c r="I25" s="1">
+        <v>4</v>
+      </c>
+      <c r="J25" s="1">
+        <v>0</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+      <c r="L25" s="1">
+        <v>16</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:S24" xr:uid="{245BFB69-89F1-144B-8F25-181FC79C8FC1}">
+    <sortState ref="A2:S25">
+      <sortCondition ref="R1:R25"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Major model improvement - stable weights embeddings initialization (he normal). Added ratings scaling in the end - sigmoid with min-max scaling
</commit_message>
<xml_diff>
--- a/notebooks/params.xlsx
+++ b/notebooks/params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/filipwojcik/projects/deepautorec_paper/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCE553B-B301-EA40-9CC9-7E7DD50DFE2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{977C63C4-1F8A-A843-8BEA-1E4710EC2093}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="params" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$S$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">params!$A$1:$T$26</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="79">
   <si>
     <t>inputs dense</t>
   </si>
@@ -233,6 +233,33 @@
   </si>
   <si>
     <t>0.386748</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>l2</t>
+  </si>
+  <si>
+    <t>0.3843</t>
+  </si>
+  <si>
+    <t>embed init</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>he normal</t>
+  </si>
+  <si>
+    <t>minmax scaling on output</t>
+  </si>
+  <si>
+    <t>0.3727</t>
+  </si>
+  <si>
+    <t>0.3829</t>
   </si>
 </sst>
 </file>
@@ -746,7 +773,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -771,6 +798,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1127,21 +1160,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:T27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="45.1640625" style="1" customWidth="1"/>
-    <col min="2" max="15" width="10.83203125" style="1"/>
-    <col min="16" max="16" width="12.33203125" style="1" customWidth="1"/>
-    <col min="17" max="19" width="10.83203125" style="1"/>
+    <col min="2" max="16" width="10.83203125" style="1"/>
+    <col min="17" max="17" width="12.33203125" style="1" customWidth="1"/>
+    <col min="18" max="19" width="10.83203125" style="1"/>
+    <col min="20" max="20" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
@@ -1161,46 +1195,49 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>44</v>
       </c>
@@ -1220,40 +1257,43 @@
         <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="4">
-        <v>16</v>
-      </c>
       <c r="I2" s="4">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
+        <v>16</v>
+      </c>
+      <c r="J2" s="4">
+        <v>8</v>
       </c>
       <c r="K2" s="1">
         <v>0</v>
       </c>
       <c r="L2" s="1">
-        <v>16</v>
-      </c>
-      <c r="N2" s="1">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>16</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -1273,40 +1313,43 @@
         <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="1">
-        <v>8</v>
-      </c>
       <c r="I3" s="1">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1">
         <v>4</v>
       </c>
-      <c r="J3" s="1">
-        <v>0</v>
-      </c>
       <c r="K3" s="1">
         <v>0</v>
       </c>
       <c r="L3" s="1">
-        <v>16</v>
-      </c>
-      <c r="N3" s="1">
-        <v>0</v>
-      </c>
-      <c r="O3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>16</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="R3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>45</v>
       </c>
@@ -1326,40 +1369,43 @@
         <v>50</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="1">
-        <v>8</v>
-      </c>
       <c r="I4" s="1">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1">
         <v>4</v>
       </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
       <c r="K4" s="1">
         <v>0</v>
       </c>
       <c r="L4" s="1">
-        <v>16</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
-      <c r="O4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>16</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="Q4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="R4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -1379,43 +1425,46 @@
         <v>50</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="1">
-        <v>8</v>
-      </c>
       <c r="I5" s="1">
+        <v>8</v>
+      </c>
+      <c r="J5" s="1">
         <v>4</v>
       </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
       <c r="K5" s="1">
         <v>0</v>
       </c>
       <c r="L5" s="1">
-        <v>16</v>
-      </c>
-      <c r="M5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>16</v>
+      </c>
+      <c r="N5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="O5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="Q5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>45</v>
       </c>
@@ -1435,40 +1484,43 @@
         <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="1">
-        <v>8</v>
-      </c>
       <c r="I6" s="1">
+        <v>8</v>
+      </c>
+      <c r="J6" s="1">
         <v>4</v>
       </c>
-      <c r="J6" s="1">
-        <v>0</v>
-      </c>
       <c r="K6" s="1">
         <v>0</v>
       </c>
       <c r="L6" s="1">
-        <v>16</v>
-      </c>
-      <c r="N6" s="1">
-        <v>0</v>
-      </c>
-      <c r="O6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M6" s="1">
+        <v>16</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -1488,40 +1540,43 @@
         <v>30</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="1">
-        <v>8</v>
-      </c>
       <c r="I7" s="1">
+        <v>8</v>
+      </c>
+      <c r="J7" s="1">
         <v>4</v>
       </c>
-      <c r="J7" s="1">
-        <v>0</v>
-      </c>
       <c r="K7" s="1">
         <v>0</v>
       </c>
       <c r="L7" s="1">
-        <v>16</v>
-      </c>
-      <c r="N7" s="1">
-        <v>0</v>
-      </c>
-      <c r="O7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="1">
+        <v>16</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="Q7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="R7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="S7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>45</v>
       </c>
@@ -1541,43 +1596,46 @@
         <v>15</v>
       </c>
       <c r="G8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H8" s="1">
-        <v>8</v>
-      </c>
       <c r="I8" s="1">
+        <v>8</v>
+      </c>
+      <c r="J8" s="1">
         <v>4</v>
       </c>
-      <c r="J8" s="1">
-        <v>0</v>
-      </c>
       <c r="K8" s="1">
         <v>0</v>
       </c>
       <c r="L8" s="1">
-        <v>16</v>
-      </c>
-      <c r="M8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>16</v>
+      </c>
+      <c r="N8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="O8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="P8" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="Q8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="R8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="S8" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>45</v>
       </c>
@@ -1597,40 +1655,43 @@
         <v>30</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="1">
-        <v>8</v>
-      </c>
       <c r="I9" s="1">
+        <v>8</v>
+      </c>
+      <c r="J9" s="1">
         <v>4</v>
       </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
       <c r="K9" s="1">
         <v>0</v>
       </c>
       <c r="L9" s="1">
-        <v>16</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>16</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q9" s="1" t="s">
+      <c r="R9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="S9" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1650,43 +1711,46 @@
         <v>15</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H10" s="1">
-        <v>8</v>
-      </c>
       <c r="I10" s="1">
+        <v>8</v>
+      </c>
+      <c r="J10" s="1">
         <v>4</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K10" s="1">
         <v>2</v>
       </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
       <c r="L10" s="1">
-        <v>16</v>
-      </c>
-      <c r="M10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1">
+        <v>16</v>
+      </c>
+      <c r="N10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="O10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="P10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="Q10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="R10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="S10" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1706,40 +1770,43 @@
         <v>30</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="1">
-        <v>8</v>
-      </c>
       <c r="I11" s="1">
+        <v>8</v>
+      </c>
+      <c r="J11" s="1">
         <v>4</v>
       </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
       <c r="K11" s="1">
         <v>0</v>
       </c>
       <c r="L11" s="1">
+        <v>0</v>
+      </c>
+      <c r="M11" s="1">
         <v>32</v>
       </c>
-      <c r="N11" s="1">
-        <v>0</v>
-      </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="Q11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="R11" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="S11" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
@@ -1758,44 +1825,47 @@
       <c r="F12" s="1">
         <v>30</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="H12" s="6">
-        <v>16</v>
-      </c>
       <c r="I12" s="6">
-        <v>8</v>
-      </c>
-      <c r="J12" s="1">
-        <v>0</v>
-      </c>
-      <c r="K12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="6">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L12" s="1">
-        <v>16</v>
-      </c>
-      <c r="M12" s="4" t="s">
+      <c r="M12" s="1">
+        <v>16</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="4" t="s">
+      <c r="O12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="Q12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="R12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="S12" s="1" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>44</v>
       </c>
@@ -1814,42 +1884,45 @@
       <c r="F13" s="6">
         <v>30</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="4">
         <v>32</v>
       </c>
-      <c r="I13" s="4">
-        <v>16</v>
-      </c>
-      <c r="J13" s="6">
-        <v>0</v>
+      <c r="J13" s="4">
+        <v>16</v>
       </c>
       <c r="K13" s="6">
         <v>0</v>
       </c>
       <c r="L13" s="6">
-        <v>16</v>
-      </c>
-      <c r="M13" s="6"/>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M13" s="6">
+        <v>16</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6">
+        <v>0</v>
+      </c>
+      <c r="P13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="P13" s="6" t="s">
+      <c r="Q13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="S13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>45</v>
       </c>
@@ -1869,13 +1942,13 @@
         <v>15</v>
       </c>
       <c r="G14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H14" s="1">
-        <v>8</v>
-      </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J14" s="1">
         <v>0</v>
@@ -1884,28 +1957,31 @@
         <v>0</v>
       </c>
       <c r="L14" s="1">
-        <v>16</v>
-      </c>
-      <c r="M14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M14" s="1">
+        <v>16</v>
+      </c>
+      <c r="N14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N14" s="1" t="s">
+      <c r="O14" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="1" t="s">
+      <c r="P14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P14" s="1" t="s">
+      <c r="Q14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q14" s="1" t="s">
+      <c r="R14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R14" s="1" t="s">
+      <c r="S14" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>45</v>
       </c>
@@ -1925,43 +2001,46 @@
         <v>100</v>
       </c>
       <c r="G15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="1">
-        <v>8</v>
-      </c>
       <c r="I15" s="1">
+        <v>8</v>
+      </c>
+      <c r="J15" s="1">
         <v>4</v>
       </c>
-      <c r="J15" s="1">
-        <v>0</v>
-      </c>
       <c r="K15" s="1">
         <v>0</v>
       </c>
       <c r="L15" s="1">
-        <v>16</v>
-      </c>
-      <c r="M15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M15" s="1">
+        <v>16</v>
+      </c>
+      <c r="N15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q15" s="1" t="s">
+      <c r="R15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R15" s="1" t="s">
+      <c r="S15" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
@@ -1980,42 +2059,45 @@
       <c r="F16" s="6">
         <v>30</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H16" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H16" s="6">
-        <v>16</v>
-      </c>
       <c r="I16" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J16" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K16" s="6">
         <v>0</v>
       </c>
       <c r="L16" s="6">
-        <v>16</v>
-      </c>
-      <c r="M16" s="6"/>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
-      <c r="O16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M16" s="6">
+        <v>16</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6">
+        <v>0</v>
+      </c>
+      <c r="P16" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P16" s="6" t="s">
+      <c r="Q16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="R16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="S16" s="1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>44</v>
       </c>
@@ -2034,42 +2116,45 @@
       <c r="F17" s="6">
         <v>30</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="G17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H17" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H17" s="6">
+      <c r="I17" s="6">
         <v>32</v>
       </c>
-      <c r="I17" s="6">
-        <v>16</v>
-      </c>
       <c r="J17" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K17" s="6">
         <v>0</v>
       </c>
       <c r="L17" s="6">
-        <v>16</v>
-      </c>
-      <c r="M17" s="6"/>
-      <c r="N17" s="6">
-        <v>0</v>
-      </c>
-      <c r="O17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M17" s="6">
+        <v>16</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6">
+        <v>0</v>
+      </c>
+      <c r="P17" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="P17" s="6" t="s">
+      <c r="Q17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="R17" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="S17" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>44</v>
       </c>
@@ -2088,42 +2173,45 @@
       <c r="F18" s="6">
         <v>30</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="6">
+      <c r="I18" s="6">
         <v>32</v>
       </c>
-      <c r="I18" s="6">
-        <v>16</v>
-      </c>
       <c r="J18" s="6">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="K18" s="6">
         <v>0</v>
       </c>
       <c r="L18" s="6">
-        <v>16</v>
-      </c>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6">
-        <v>0</v>
-      </c>
-      <c r="O18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="6">
+        <v>16</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6">
+        <v>0</v>
+      </c>
+      <c r="P18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="P18" s="6" t="s">
+      <c r="Q18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="R18" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="S18" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
@@ -2142,42 +2230,45 @@
       <c r="F19" s="6">
         <v>30</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H19" s="6">
-        <v>16</v>
-      </c>
       <c r="I19" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J19" s="6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K19" s="6">
         <v>0</v>
       </c>
       <c r="L19" s="6">
-        <v>16</v>
-      </c>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6">
-        <v>0</v>
-      </c>
-      <c r="O19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="M19" s="6">
+        <v>16</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6">
+        <v>0</v>
+      </c>
+      <c r="P19" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="P19" s="6" t="s">
+      <c r="Q19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q19" s="1" t="s">
+      <c r="R19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="R19" s="1" t="s">
+      <c r="S19" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>45</v>
       </c>
@@ -2197,43 +2288,46 @@
         <v>15</v>
       </c>
       <c r="G20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H20" s="1">
-        <v>16</v>
-      </c>
       <c r="I20" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
       </c>
       <c r="L20" s="1">
-        <v>16</v>
-      </c>
-      <c r="M20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M20" s="1">
+        <v>16</v>
+      </c>
+      <c r="N20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="O20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="P20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="R20" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="S20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>44</v>
       </c>
@@ -2252,42 +2346,45 @@
       <c r="F21" s="6">
         <v>30</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="1">
+      <c r="I21" s="1">
         <v>32</v>
       </c>
-      <c r="I21" s="1">
-        <v>16</v>
-      </c>
-      <c r="J21" s="6">
-        <v>0</v>
+      <c r="J21" s="1">
+        <v>16</v>
       </c>
       <c r="K21" s="6">
         <v>0</v>
       </c>
       <c r="L21" s="6">
-        <v>16</v>
-      </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6">
-        <v>0</v>
-      </c>
-      <c r="O21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>16</v>
+      </c>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6">
+        <v>0</v>
+      </c>
+      <c r="P21" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="P21" s="6" t="s">
+      <c r="Q21" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="R21" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="S21" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
@@ -2307,40 +2404,43 @@
         <v>30</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="6">
-        <v>16</v>
-      </c>
       <c r="I22" s="6">
-        <v>8</v>
-      </c>
-      <c r="J22" s="1">
-        <v>0</v>
-      </c>
-      <c r="K22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="6">
+        <v>8</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0</v>
+      </c>
+      <c r="L22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L22" s="1">
-        <v>16</v>
-      </c>
-      <c r="N22" s="1">
-        <v>0</v>
-      </c>
-      <c r="O22" s="1" t="s">
+      <c r="M22" s="1">
+        <v>16</v>
+      </c>
+      <c r="O22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="R22" s="1" t="s">
+      <c r="S22" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>44</v>
       </c>
@@ -2360,40 +2460,43 @@
         <v>30</v>
       </c>
       <c r="G23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="6">
-        <v>16</v>
-      </c>
       <c r="I23" s="6">
-        <v>8</v>
-      </c>
-      <c r="J23" s="1">
-        <v>0</v>
-      </c>
-      <c r="K23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23" s="6">
+        <v>8</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0</v>
+      </c>
+      <c r="L23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="L23" s="1">
-        <v>16</v>
-      </c>
-      <c r="N23" s="1">
-        <v>0</v>
-      </c>
-      <c r="O23" s="1" t="s">
+      <c r="M23" s="1">
+        <v>16</v>
+      </c>
+      <c r="O23" s="1">
+        <v>0</v>
+      </c>
+      <c r="P23" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q23" s="1" t="s">
+      <c r="R23" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="R23" s="1" t="s">
+      <c r="S23" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>45</v>
       </c>
@@ -2413,43 +2516,46 @@
         <v>15</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="1">
+      <c r="I24" s="1">
         <v>4</v>
       </c>
-      <c r="I24" s="1">
+      <c r="J24" s="1">
         <v>2</v>
       </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
       <c r="K24" s="1">
         <v>0</v>
       </c>
       <c r="L24" s="1">
-        <v>16</v>
-      </c>
-      <c r="M24" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M24" s="1">
+        <v>16</v>
+      </c>
+      <c r="N24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N24" s="1" t="s">
+      <c r="O24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="P24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q24" s="1" t="s">
+      <c r="R24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R24" s="1" t="s">
+      <c r="S24" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>45</v>
       </c>
@@ -2469,46 +2575,170 @@
         <v>15</v>
       </c>
       <c r="G25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="1">
-        <v>16</v>
-      </c>
       <c r="I25" s="1">
+        <v>16</v>
+      </c>
+      <c r="J25" s="1">
         <v>4</v>
       </c>
-      <c r="J25" s="1">
-        <v>0</v>
-      </c>
       <c r="K25" s="1">
         <v>0</v>
       </c>
       <c r="L25" s="1">
-        <v>16</v>
-      </c>
-      <c r="M25" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M25" s="1">
+        <v>16</v>
+      </c>
+      <c r="N25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N25" s="1" t="s">
+      <c r="O25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="P25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="P25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Q25" s="1" t="s">
+      <c r="R25" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R25" s="1" t="s">
+      <c r="S25" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="1">
+        <v>32</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1">
+        <v>30</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I26" s="1">
+        <v>16</v>
+      </c>
+      <c r="J26" s="1">
+        <v>8</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M26" s="1">
+        <v>16</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O26" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R26" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="51" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" s="1">
+        <v>32</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1">
+        <v>30</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I27" s="1">
+        <v>16</v>
+      </c>
+      <c r="J27" s="1">
+        <v>8</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="M27" s="1">
+        <v>16</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="O27" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R27" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="S27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="T27" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S24" xr:uid="{245BFB69-89F1-144B-8F25-181FC79C8FC1}">
-    <sortState ref="A2:S25">
-      <sortCondition ref="R1:R25"/>
+  <autoFilter ref="A1:T26" xr:uid="{245BFB69-89F1-144B-8F25-181FC79C8FC1}">
+    <sortState ref="A2:T25">
+      <sortCondition ref="S1:S25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>